<commit_message>
refactor: handle inconsistent conainer error
</commit_message>
<xml_diff>
--- a/tests/tests_unit/rules/test_importers/data/inconsistent_container_dms_rules.xlsx
+++ b/tests/tests_unit/rules/test_importers/data/inconsistent_container_dms_rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndersAlbert\Projects\internal\neat\tests\tests_unit\rules\test_importers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E29594D-927C-491C-87B7-BF8E2429626D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B747A895-0B2C-4E45-83E2-3569C0FE33A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41172" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:W1000"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9555,10 +9555,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:W1008"/>
+  <dimension ref="A1:W1006"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9699,6 +9699,33 @@
       <c r="W3" s="10"/>
     </row>
     <row r="4" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>39</v>
+      </c>
       <c r="R4" s="10"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
@@ -9706,13 +9733,13 @@
     </row>
     <row r="5" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -9727,15 +9754,11 @@
         <v>39</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="M5" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
     </row>
     <row r="6" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="R6" s="10"/>
@@ -9744,48 +9767,25 @@
       <c r="U6" s="10"/>
     </row>
     <row r="7" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L7" t="s">
-        <v>42</v>
-      </c>
-      <c r="M7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="R8" s="10"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-    </row>
-    <row r="9" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="R9" s="10"/>
-      <c r="S9" s="10"/>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-    </row>
-    <row r="10" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="10"/>
+      <c r="U7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="R10" s="10"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="R11" s="10"/>
+      <c r="S11" s="10"/>
+      <c r="T11" s="10"/>
+      <c r="U11" s="10"/>
+    </row>
     <row r="12" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
@@ -9804,49 +9804,49 @@
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-    </row>
+    <row r="15" spans="1:23" ht="14.4" x14ac:dyDescent="0.3"/>
     <row r="16" spans="1:23" ht="14.4" x14ac:dyDescent="0.3">
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
     </row>
-    <row r="17" spans="18:21" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="18:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+    </row>
     <row r="18" spans="18:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
     </row>
-    <row r="19" spans="18:21" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-    </row>
-    <row r="20" spans="18:21" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="18:21" ht="14.4" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
     </row>
-    <row r="21" spans="18:21" ht="14.4" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-    </row>
+    <row r="21" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+    </row>
+    <row r="22" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R23" s="10"/>
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
     </row>
-    <row r="24" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R24" s="10"/>
+      <c r="S24" s="10"/>
+      <c r="T24" s="10"/>
+      <c r="U24" s="10"/>
+    </row>
     <row r="25" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R25" s="10"/>
       <c r="S25" s="10"/>
@@ -9854,14 +9854,14 @@
       <c r="U25" s="10"/>
     </row>
     <row r="26" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
       <c r="T26" s="10"/>
       <c r="U26" s="10"/>
     </row>
     <row r="27" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
     </row>
@@ -9877,66 +9877,62 @@
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>
     </row>
-    <row r="30" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="10"/>
-      <c r="U30" s="10"/>
-    </row>
+    <row r="30" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R31" s="11"/>
+      <c r="R31" s="10"/>
       <c r="S31" s="11"/>
       <c r="T31" s="10"/>
       <c r="U31" s="10"/>
     </row>
-    <row r="32" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="10"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="10"/>
+      <c r="U32" s="10"/>
+    </row>
+    <row r="33" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R33" s="10"/>
       <c r="S33" s="11"/>
       <c r="T33" s="10"/>
       <c r="U33" s="10"/>
     </row>
-    <row r="34" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R34" s="10"/>
       <c r="S34" s="11"/>
       <c r="T34" s="10"/>
       <c r="U34" s="10"/>
     </row>
-    <row r="35" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="R35" s="10"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-    </row>
-    <row r="36" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R36" s="10"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="10"/>
-      <c r="U36" s="10"/>
-    </row>
-    <row r="37" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R37" s="10"/>
-    </row>
-    <row r="38" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="18:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="36" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C47" s="12"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+    </row>
+    <row r="48" spans="3:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+    </row>
     <row r="49" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="12"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="K49" s="9"/>
-      <c r="L49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
     </row>
     <row r="50" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N50" s="9"/>
@@ -9963,10 +9959,28 @@
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C56" s="12"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
       <c r="N56" s="9"/>
       <c r="O56" s="9"/>
     </row>
     <row r="57" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="12"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
       <c r="N57" s="9"/>
       <c r="O57" s="9"/>
     </row>
@@ -22306,32 +22320,6 @@
       <c r="M1006" s="9"/>
       <c r="N1006" s="9"/>
       <c r="O1006" s="9"/>
-    </row>
-    <row r="1007" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1007" s="12"/>
-      <c r="F1007" s="9"/>
-      <c r="G1007" s="9"/>
-      <c r="H1007" s="9"/>
-      <c r="I1007" s="9"/>
-      <c r="J1007" s="9"/>
-      <c r="K1007" s="9"/>
-      <c r="L1007" s="9"/>
-      <c r="M1007" s="9"/>
-      <c r="N1007" s="9"/>
-      <c r="O1007" s="9"/>
-    </row>
-    <row r="1008" spans="3:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1008" s="12"/>
-      <c r="F1008" s="9"/>
-      <c r="G1008" s="9"/>
-      <c r="H1008" s="9"/>
-      <c r="I1008" s="9"/>
-      <c r="J1008" s="9"/>
-      <c r="K1008" s="9"/>
-      <c r="L1008" s="9"/>
-      <c r="M1008" s="9"/>
-      <c r="N1008" s="9"/>
-      <c r="O1008" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>